<commit_message>
changes the soft skills input type and the reasoning chain
</commit_message>
<xml_diff>
--- a/main/results/1.xlsx
+++ b/main/results/1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,16 +475,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>85.02</v>
+        <v>87.69</v>
       </c>
       <c r="D2" t="n">
         <v>0.9</v>
       </c>
       <c r="E2" t="n">
-        <v>76.52</v>
+        <v>78.92</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -493,20 +493,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CloudPhysician's Vital Extraction Challenge</t>
+          <t>Multi Model Data Analysis for Annotation of Human Activities</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>78.28</v>
       </c>
       <c r="D3" t="n">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>78.28</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -515,64 +515,64 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Multi Model Data Analysis for Annotation of Human Activities</t>
+          <t>CloudPhysician's Vital Extraction Challenge</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>63.75</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LLMGuard</t>
+          <t>SMART SENSING MIDDLEWARE</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>87.69</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>87.69</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RAPID</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>81.62</v>
+      </c>
+      <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>FaceNet Implementation</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.85</v>
-      </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>81.62</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -581,17 +581,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RAPID</t>
+          <t>SHAMIYANA APP</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>87.69</v>
+        <v>78.28</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E7" t="n">
-        <v>87.69</v>
+        <v>70.45</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
@@ -599,134 +599,46 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SMART SENSING MIDDLEWARE</t>
+          <t>Website for the Literature Society of the college</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>87.69</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E8" t="n">
-        <v>87.69</v>
+        <v>78.92</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>LLMGuard</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>78.28</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>78.28</v>
+      </c>
+      <c r="F9" t="n">
         <v>2</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SHAMIYANA APP</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>75</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E9" t="n">
-        <v>67.5</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>3</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Website for the Literature Society of the college</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>85.02</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E10" t="n">
-        <v>76.52</v>
-      </c>
-      <c r="F10" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>LLMGuard</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>78.28</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>78.28</v>
-      </c>
-      <c r="F11" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Multi Model Data Analysis for Annotation of Human Activities</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>75</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>75</v>
-      </c>
-      <c r="F12" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Cloudphysician's Vital Extraction Challenge</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>